<commit_message>
Updating histology and sequencing metadata
</commit_message>
<xml_diff>
--- a/10x-multiome/latest/10x-multiome.xlsx
+++ b/10x-multiome/latest/10x-multiome.xlsx
@@ -60,7 +60,7 @@
     <comment ref="E1" authorId="1">
       <text>
         <t>(Required) The path to the file with the ORCID IDs for all contributors of this
-dataset (e.g., "extras/contributors.tsv" or "./contributors.tsv"). This is an
+dataset (e.g., "./extras/contributors.tsv" or "./contributors.tsv"). This is an
 internal metadata field that is just used for ingest.</t>
       </text>
     </comment>
@@ -70,8 +70,8 @@
 a single dataset upload this might be "." where as for a data upload containing
 multiple datasets, this would be the directory name for the respective dataset.
 For instance, if the data is within a directory called "TEST001-RK" use syntax
-"/TEST001-RK/" for this field. If there are multiple directory levels, use the
-format "/TEST001-RK/Run1/Pass2" in which "Pass2" is the subdirectory where the
+"./TEST001-RK" for this field. If there are multiple directory levels, use the
+format "./TEST001-RK/Run1/Pass2" in which "Pass2" is the subdirectory where the
 single dataset's data is stored. This is an internal metadata field that is just
 used for ingest.</t>
       </text>
@@ -502,7 +502,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-10-05T09:35:16-07:00</t>
+    <t>2023-10-06T19:20:00-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>

</xml_diff>

<commit_message>
Minor update on sequencing assays
</commit_message>
<xml_diff>
--- a/10x-multiome/latest/10x-multiome.xlsx
+++ b/10x-multiome/latest/10x-multiome.xlsx
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="136">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -157,6 +157,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000246</t>
   </si>
   <si>
+    <t>MIBI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
+  </si>
+  <si>
     <t>DESI</t>
   </si>
   <si>
@@ -217,12 +223,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000222</t>
   </si>
   <si>
-    <t>Multiplex Ion Beam Imaging</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
-  </si>
-  <si>
     <t>SIMS</t>
   </si>
   <si>
@@ -367,6 +367,24 @@
     <t>preparation_instrument_vendor</t>
   </si>
   <si>
+    <t>Leica Biosystems</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023603</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C48660</t>
+  </si>
+  <si>
+    <t>HTX Technologies</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023734</t>
+  </si>
+  <si>
     <t>10x Genomics</t>
   </si>
   <si>
@@ -379,16 +397,10 @@
     <t>https://identifiers.org/RRID:SCR_017105</t>
   </si>
   <si>
-    <t>Not applicable</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C48660</t>
-  </si>
-  <si>
-    <t>HTX Technologies</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023734</t>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C126386</t>
   </si>
   <si>
     <t>SunChrom</t>
@@ -400,22 +412,52 @@
     <t>preparation_instrument_model</t>
   </si>
   <si>
+    <t>NanoZoomer S210</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023760</t>
+  </si>
+  <si>
+    <t>Sublimator</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023729</t>
+  </si>
+  <si>
+    <t>Chromium Controller</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_019326</t>
+  </si>
+  <si>
+    <t>NanoZoomer S360</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023761</t>
+  </si>
+  <si>
+    <t>NanoZoomer S60</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023762</t>
+  </si>
+  <si>
     <t>Chromium X</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_024537</t>
   </si>
   <si>
-    <t>NanoZoomer S210</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023760</t>
-  </si>
-  <si>
-    <t>Sublimator</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023729</t>
+    <t>AutoStainer XL</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023957</t>
+  </si>
+  <si>
+    <t>Visium CytAssist</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024570</t>
   </si>
   <si>
     <t>SunCollect Sprayer</t>
@@ -430,12 +472,6 @@
     <t>https://identifiers.org/RRID:SCR_023731</t>
   </si>
   <si>
-    <t>Chromium Controller</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_019326</t>
-  </si>
-  <si>
     <t>Chromium iX</t>
   </si>
   <si>
@@ -454,18 +490,6 @@
     <t>https://identifiers.org/RRID:SCR_023732</t>
   </si>
   <si>
-    <t>NanoZoomer S360</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023761</t>
-  </si>
-  <si>
-    <t>NanoZoomer S60</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023762</t>
-  </si>
-  <si>
     <t>preparation_instrument_kit</t>
   </si>
   <si>
@@ -502,7 +526,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-10-06T19:20:00-07:00</t>
+    <t>2023-10-20T15:01:07-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -634,21 +658,21 @@
         <v>79</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2">
       <c r="L2" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -657,10 +681,10 @@
       <formula1>'dataset_type'!$A$1:$A$36</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_vendor'!$A$1:$A$5</formula1>
+      <formula1>'preparation_instrument_vendor'!$A$1:$A$7</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_model'!$A$1:$A$12</formula1>
+      <formula1>'preparation_instrument_model'!$A$1:$A$14</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="J2:J1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_instrument_kit'!$A$1:$A$2</formula1>
@@ -979,7 +1003,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1025,6 +1049,22 @@
         <v>89</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1032,7 +1072,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1040,98 +1080,114 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B11" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1149,18 +1205,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1184,16 +1240,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="C1" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="D1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2">
@@ -1201,13 +1257,13 @@
         <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating ID pattern to accept SenNet ID
</commit_message>
<xml_diff>
--- a/10x-multiome/latest/10x-multiome.xlsx
+++ b/10x-multiome/latest/10x-multiome.xlsx
@@ -25,11 +25,12 @@
   <commentList>
     <comment ref="A1" authorId="1">
       <text>
-        <t>(Required) HuBMAP ID of the sample (i.e., block, section or suspension) used to
-perform this assay. For example, for a RNAseq assay, the parent would be the
-suspension, whereas this would be the HuBMAP ID of a section for one of the
-imaging assays. If an assay comes from multiple parent samples then this should
-be a comma separated list. Example: HBM765.TRHD.452</t>
+        <t>(Required) Unique HuBMAP or SenNet identifier of the sample (i.e., block,
+section or suspension) used to perform this assay. For example, for a RNAseq
+assay, the parent would be the suspension, whereas, for one of the imaging
+assays, the parent would be the tissue section. If an assay comes from multiple
+parent samples then this should be a comma separated list. Example:
+HBM386.ZGKG.235, HBM672.MKPK.442 or SNT232.UBHJ.322, SNT329.ALSK.102</t>
       </text>
     </comment>
     <comment ref="B1" authorId="1">
@@ -526,7 +527,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-10-20T19:59:16-07:00</t>
+    <t>2023-10-27T18:08:17-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>

</xml_diff>

<commit_message>
Updated all assays to accommodate the newly introduced dataset type
</commit_message>
<xml_diff>
--- a/10x-multiome/latest/10x-multiome.xlsx
+++ b/10x-multiome/latest/10x-multiome.xlsx
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="134">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -152,12 +152,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
   </si>
   <si>
-    <t>nanoPOTS</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000246</t>
-  </si>
-  <si>
     <t>MIBI</t>
   </si>
   <si>
@@ -260,12 +254,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
   </si>
   <si>
-    <t>NanoDESI</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000203</t>
-  </si>
-  <si>
     <t>GeoMx</t>
   </si>
   <si>
@@ -284,6 +272,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000201</t>
   </si>
   <si>
+    <t>2D Imaging Mass Cytometry</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000296</t>
+  </si>
+  <si>
     <t>RNAseq (GeoMx)</t>
   </si>
   <si>
@@ -527,7 +521,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-10-27T18:08:17-07:00</t>
+    <t>2023-11-02T15:45:13-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -647,39 +641,39 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s" s="1">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s" s="1">
         <v>76</v>
       </c>
-      <c r="F1" t="s" s="1">
+      <c r="H1" t="s" s="1">
         <v>77</v>
       </c>
-      <c r="G1" t="s" s="1">
-        <v>78</v>
-      </c>
-      <c r="H1" t="s" s="1">
-        <v>79</v>
-      </c>
       <c r="I1" t="s" s="1">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2">
       <c r="L2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$36</formula1>
+      <formula1>'dataset_type'!$A$1:$A$35</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_instrument_vendor'!$A$1:$A$7</formula1>
@@ -703,7 +697,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -987,14 +981,6 @@
       </c>
       <c r="B35" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1012,58 +998,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1081,114 +1067,114 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1206,18 +1192,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1241,30 +1227,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" t="s">
         <v>130</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>132</v>
-      </c>
-      <c r="D1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" t="s">
         <v>131</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>133</v>
-      </c>
-      <c r="D2" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update all assays to have a default dataset_type value
</commit_message>
<xml_diff>
--- a/10x-multiome/latest/10x-multiome.xlsx
+++ b/10x-multiome/latest/10x-multiome.xlsx
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="130">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -158,18 +158,18 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
   </si>
   <si>
+    <t>Visium (no probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
+  </si>
+  <si>
     <t>DESI</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
   </si>
   <si>
-    <t>scATACseq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000247</t>
-  </si>
-  <si>
     <t>Auto-fluorescence</t>
   </si>
   <si>
@@ -182,22 +182,16 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
   </si>
   <si>
-    <t>scRNAseq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000248</t>
-  </si>
-  <si>
     <t>Xenium</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000219</t>
   </si>
   <si>
-    <t>snATACseq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000183</t>
+    <t>Visium (with probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
   </si>
   <si>
     <t>Molecular Cartography</t>
@@ -224,12 +218,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000202</t>
   </si>
   <si>
-    <t>RNAseq (Visium)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000188</t>
-  </si>
-  <si>
     <t>Cell DIVE</t>
   </si>
   <si>
@@ -242,6 +230,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000160</t>
   </si>
   <si>
+    <t>GeoMx (NGS)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000300</t>
+  </si>
+  <si>
     <t>CyCIF</t>
   </si>
   <si>
@@ -254,18 +248,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
   </si>
   <si>
-    <t>GeoMx</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000216</t>
-  </si>
-  <si>
-    <t>RNAseq (bulk)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000212</t>
-  </si>
-  <si>
     <t>MALDI</t>
   </si>
   <si>
@@ -278,10 +260,10 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000296</t>
   </si>
   <si>
-    <t>RNAseq (GeoMx)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000214</t>
+    <t>ATACseq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
   </si>
   <si>
     <t>Histology</t>
@@ -296,10 +278,10 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000209</t>
   </si>
   <si>
-    <t>ATACseq (bulk)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000210</t>
+    <t>RNAseq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000310</t>
   </si>
   <si>
     <t>MERFISH</t>
@@ -314,12 +296,30 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000194</t>
   </si>
   <si>
+    <t>nanoSPLITS</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000312</t>
+  </si>
+  <si>
     <t>10X Multiome</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
   </si>
   <si>
+    <t>GeoMx (nCounter)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000301</t>
+  </si>
+  <si>
+    <t>RNAseq (with probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000311</t>
+  </si>
+  <si>
     <t>PhenoCycler</t>
   </si>
   <si>
@@ -338,18 +338,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
   </si>
   <si>
-    <t>snRNAseq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000184</t>
-  </si>
-  <si>
-    <t>Visium</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000187</t>
-  </si>
-  <si>
     <t>contributors_path</t>
   </si>
   <si>
@@ -521,7 +509,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-11-07T20:05:33-08:00</t>
+    <t>2023-11-15T17:13:38-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -641,39 +629,42 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2">
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
       <c r="L2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$35</formula1>
+      <formula1>'dataset_type'!$A$1:$A$33</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_instrument_vendor'!$A$1:$A$7</formula1>
@@ -697,7 +688,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -965,22 +956,6 @@
       </c>
       <c r="B33" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>70</v>
-      </c>
-      <c r="B34" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -998,58 +973,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1067,114 +1042,114 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B12" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1192,18 +1167,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1227,30 +1202,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" t="s">
         <v>128</v>
-      </c>
-      <c r="C1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" t="s">
         <v>129</v>
-      </c>
-      <c r="C2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D2" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added "Custom" as an option for any experiment kits
Closes #43
</commit_message>
<xml_diff>
--- a/10x-multiome/latest/10x-multiome.xlsx
+++ b/10x-multiome/latest/10x-multiome.xlsx
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="164">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -188,6 +188,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000219</t>
   </si>
   <si>
+    <t>Stereo-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
+  </si>
+  <si>
     <t>Visium (with probes)</t>
   </si>
   <si>
@@ -236,6 +242,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000300</t>
   </si>
   <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
+  </si>
+  <si>
     <t>CyCIF</t>
   </si>
   <si>
@@ -278,6 +290,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000209</t>
   </si>
   <si>
+    <t>Resolve</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000384</t>
+  </si>
+  <si>
     <t>RNAseq</t>
   </si>
   <si>
@@ -368,6 +386,18 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C48660</t>
   </si>
   <si>
+    <t>Thermo Fisher Scientific</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_008452</t>
+  </si>
+  <si>
+    <t>Roche Diagnostics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025096</t>
+  </si>
+  <si>
     <t>HTX Technologies</t>
   </si>
   <si>
@@ -407,6 +437,12 @@
     <t>https://identifiers.org/RRID:SCR_023729</t>
   </si>
   <si>
+    <t>EVOS M7000</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025070</t>
+  </si>
+  <si>
     <t>Chromium Controller</t>
   </si>
   <si>
@@ -455,12 +491,30 @@
     <t>https://identifiers.org/RRID:SCR_023731</t>
   </si>
   <si>
+    <t>Discovery Ultra</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025097</t>
+  </si>
+  <si>
+    <t>ST5020 Multistainer</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025021</t>
+  </si>
+  <si>
     <t>Chromium iX</t>
   </si>
   <si>
     <t>https://identifiers.org/RRID:SCR_024536</t>
   </si>
   <si>
+    <t>Chromium Connect</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025146</t>
+  </si>
+  <si>
     <t>M5 Sprayer</t>
   </si>
   <si>
@@ -476,16 +530,64 @@
     <t>preparation_instrument_kit</t>
   </si>
   <si>
+    <t>10X Genomics; Chromium Next GEM Chip G Single Cell Kit, 16 rxns; PN 1000127</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000379</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Chip K Automated Single Cell Kit, 48 rxns; PN 1000289</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000373</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium NextGem Single Cell Multiome ATAC + Gene Expression Reagent Bundle, 16 rxn; PN 1000283</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000250</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium NextGem Single Cell Multiome ATAC + Gene Expression Reagent Bundle, 4 rxn; PN 1000285</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000251</t>
   </si>
   <si>
-    <t>10X Genomics; Chromium NextGem Single Cell Multiome ATAC + Gene Expression Reagent Bundle, 16 rxn; PN 1000283</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000250</t>
+    <t>10X Genomics; Chromium Next GEM Chip K Single Cell Kit, 48 rxns; PN 1000286</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000367</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Chip G Single Cell Kit, 48 rxns; PN 1000120</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000378</t>
+  </si>
+  <si>
+    <t>10X Genomics; Visium FFPE Reagent Kit v2-Small, PN 1000436</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000324</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65167</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Chip Q Single Cell Kit, 16 rxns; PN 1000422</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000325</t>
+  </si>
+  <si>
+    <t>10X Genomics; Chromium Next GEM Chip K Single Cell Kit, 16 rxns; PN 1000287</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000368</t>
   </si>
   <si>
     <t>number_of_pre_amplification_pcr_cycles</t>
@@ -509,7 +611,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-11-24T09:44:18-08:00</t>
+    <t>2024-06-05T17:28:30-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -601,18 +703,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" style="2" width="16.6875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" style="3" width="6.33984375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" style="4" width="23.45703125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" style="5" width="12.28515625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" style="6" width="16.90625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" style="7" width="9.81640625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" style="8" width="16.19140625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" style="9" width="29.08203125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" style="10" width="28.48828125" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" style="11" width="25.23046875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" style="12" width="37.00390625" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" style="13" width="19.61328125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" style="2" width="14.39453125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" style="3" width="5.46875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" style="4" width="20.234375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" style="5" width="10.59765625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" style="6" width="14.5859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" style="7" width="8.46484375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" style="8" width="13.96484375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" style="9" width="25.0859375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" style="10" width="24.57421875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" style="11" width="21.765625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" style="12" width="31.91796875" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" style="13" width="16.91796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -629,51 +731,51 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>121</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2">
-      <c r="D2" t="s">
-        <v>58</v>
-      </c>
-      <c r="L2" t="s">
-        <v>122</v>
+      <c r="D2" t="s" s="5">
+        <v>64</v>
+      </c>
+      <c r="L2" t="s" s="13">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$33</formula1>
+      <formula1>'dataset_type'!$A$1:$A$36</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_vendor'!$A$1:$A$7</formula1>
+      <formula1>'preparation_instrument_vendor'!$A$1:$A$9</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_model'!$A$1:$A$14</formula1>
+      <formula1>'preparation_instrument_model'!$A$1:$A$18</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="J2:J1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_kit'!$A$1:$A$2</formula1>
+      <formula1>'preparation_instrument_kit'!$A$1:$A$10</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="between" sqref="K2:K1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-2147483648</formula1>
@@ -688,274 +790,298 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>27</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>29</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>31</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
         <v>33</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>35</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" t="s" s="0">
         <v>37</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>39</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" t="s" s="0">
         <v>41</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" t="s" s="0">
         <v>43</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" t="s" s="0">
         <v>45</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s">
+      <c r="A22" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" t="s" s="0">
         <v>47</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s">
+      <c r="A23" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="s" s="0">
         <v>49</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s">
+      <c r="A24" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" t="s" s="0">
         <v>51</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s">
+      <c r="A25" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" t="s" s="0">
         <v>53</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s">
+      <c r="A26" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" t="s" s="0">
         <v>55</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s">
+      <c r="A27" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" t="s" s="0">
         <v>57</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s">
+      <c r="A28" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" t="s" s="0">
         <v>59</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s">
+      <c r="A29" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" t="s" s="0">
         <v>61</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s">
+      <c r="A30" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" t="s" s="0">
         <v>63</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s">
+      <c r="A31" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" t="s" s="0">
         <v>65</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s">
+      <c r="A32" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" t="s" s="0">
         <v>67</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s">
+      <c r="A33" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" t="s" s="0">
         <v>69</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -965,66 +1091,82 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" t="s">
-        <v>75</v>
+      <c r="A1" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>81</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" t="s">
-        <v>77</v>
+      <c r="A2" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>83</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" t="s">
-        <v>79</v>
+      <c r="A3" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>85</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" t="s">
-        <v>81</v>
+      <c r="A4" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>87</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" t="s">
-        <v>83</v>
+      <c r="A5" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>89</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" t="s">
-        <v>85</v>
+      <c r="A6" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>91</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" t="s">
-        <v>87</v>
+      <c r="A7" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1034,122 +1176,154 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" t="s">
-        <v>90</v>
+      <c r="A1" t="s" s="0">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>100</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" t="s">
-        <v>79</v>
+      <c r="A2" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>85</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" t="s">
-        <v>92</v>
+      <c r="A3" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>102</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" t="s">
-        <v>94</v>
+      <c r="A4" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>104</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" t="s">
-        <v>96</v>
+      <c r="A5" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>106</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" t="s">
-        <v>98</v>
+      <c r="A6" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>108</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" t="s">
-        <v>100</v>
+      <c r="A7" t="s" s="0">
+        <v>109</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>110</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" t="s">
-        <v>102</v>
+      <c r="A8" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>112</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B9" t="s">
-        <v>104</v>
+      <c r="A9" t="s" s="0">
+        <v>113</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>114</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>105</v>
-      </c>
-      <c r="B10" t="s">
-        <v>106</v>
+      <c r="A10" t="s" s="0">
+        <v>115</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>116</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" t="s">
-        <v>108</v>
+      <c r="A11" t="s" s="0">
+        <v>117</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>118</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B12" t="s">
-        <v>110</v>
+      <c r="A12" t="s" s="0">
+        <v>119</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>120</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B13" t="s">
-        <v>112</v>
+      <c r="A13" t="s" s="0">
+        <v>121</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>122</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14" t="s">
-        <v>114</v>
+      <c r="A14" t="s" s="0">
+        <v>123</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>125</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>127</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>129</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>131</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1159,26 +1333,90 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" t="s">
-        <v>117</v>
+      <c r="A1" t="s" s="0">
+        <v>134</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>135</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" t="s">
-        <v>119</v>
+      <c r="A2" t="s" s="0">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>138</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>140</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>142</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>144</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>146</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>148</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>150</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>152</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1194,38 +1432,38 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="13.41015625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="27.9921875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="79.9765625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="11.5703125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="9.65234375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="24.1484375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="68.98828125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D1" t="s">
-        <v>128</v>
+      <c r="A1" t="s" s="0">
+        <v>157</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>158</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>160</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>162</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D2" t="s">
-        <v>129</v>
+      <c r="A2" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>159</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>161</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating analyte classes list
</commit_message>
<xml_diff>
--- a/10x-multiome/latest/10x-multiome.xlsx
+++ b/10x-multiome/latest/10x-multiome.xlsx
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="170">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -266,6 +266,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000201</t>
   </si>
   <si>
+    <t>seqFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
+  </si>
+  <si>
     <t>2D Imaging Mass Cytometry</t>
   </si>
   <si>
@@ -290,6 +296,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000209</t>
   </si>
   <si>
+    <t>DART-FISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000396</t>
+  </si>
+  <si>
     <t>Resolve</t>
   </si>
   <si>
@@ -554,6 +566,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000251</t>
   </si>
   <si>
+    <t>10x Genomics; Chromium GEM-X Single Cell 3' Kit v4, 16 rxns; PN 1000691</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000400</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium Next GEM Chip K Single Cell Kit, 48 rxns; PN 1000286</t>
   </si>
   <si>
@@ -611,7 +629,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-11-01T11:48:57-07:00</t>
+    <t>2025-01-08T12:48:31-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -731,42 +749,42 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="L2" t="s" s="13">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$36</formula1>
+      <formula1>'dataset_type'!$A$1:$A$38</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_instrument_vendor'!$A$1:$A$9</formula1>
@@ -775,7 +793,7 @@
       <formula1>'preparation_instrument_model'!$A$1:$A$18</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="J2:J1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_kit'!$A$1:$A$10</formula1>
+      <formula1>'preparation_instrument_kit'!$A$1:$A$11</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="between" sqref="K2:K1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-2147483648</formula1>
@@ -790,7 +808,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1082,6 +1100,22 @@
       </c>
       <c r="B36" t="s" s="0">
         <v>75</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1099,74 +1133,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1184,146 +1218,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1333,7 +1367,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1341,82 +1375,90 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>153</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>158</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1440,30 +1482,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update multi-assay metadata templates to use updated field descriptions
</commit_message>
<xml_diff>
--- a/10x-multiome/latest/10x-multiome.xlsx
+++ b/10x-multiome/latest/10x-multiome.xlsx
@@ -25,99 +25,102 @@
   <commentList>
     <comment ref="A1" authorId="1">
       <text>
-        <t>(Required) Unique HuBMAP or SenNet identifier of the sample (i.e., block,
-section or suspension) used to perform this assay. For example, for a RNAseq
-assay, the parent would be the suspension, whereas, for one of the imaging
-assays, the parent would be the tissue section. If an assay comes from multiple
-parent samples then this should be a comma separated list. Example:
-HBM386.ZGKG.235, HBM672.MKPK.442 or SNT232.UBHJ.322, SNT329.ALSK.102</t>
+        <t>(Required) The unique identifier from HuBMAP or SenNet for the sample (such as a
+block, section, or suspension) used to perform the assay. For instance, in an
+RNAseq assay, the parent sample would be the suspension, while in imaging
+assays, it would be the tissue section. If the assay is derived from multiple
+parent samples, this field should contain a comma-separated list of identifiers.
+Example: HBM386.ZGKG.235, HBM672.MKPK.442</t>
       </text>
     </comment>
     <comment ref="B1" authorId="1">
       <text>
-        <t>An internal field labs can use it to add whatever ID(s) they want or need for
-dataset validation and tracking. This could be a single ID (e.g.,
-"Visium_9OLC_A4_S1") or a delimited list of IDs (e.g., “9OL; 9OLC.A2;
-Visium_9OLC_A4_S1”). This field will not be accessible to anyone outside of the
-consortium and no effort will be made to check if IDs provided by one data
-provider are also used by another.</t>
+        <t>A locally assigned identifier provided by the data provider for the dataset. It
+is used to reference an external metadata record that may be maintained
+independently, enabling traceability and supporting provenance tracking.
+Example: Visium_9OLC_A4_S1</t>
       </text>
     </comment>
     <comment ref="C1" authorId="1">
       <text>
-        <t>(Required) DOI for the protocols.io page that describes the assay or sample
-procurement and preparation. For example for an imaging assay, the protocol
-might begin with staining of a section and finalize with the creation of an
-OME-TIFF file. In this case the protocol would include any image processing
-steps required to create the OME-TIFF file. Example:
-https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1.</t>
+        <t>(Required) The DOI for the protocols.io page that details the assay or the
+procedures used for sample procurement and preparation. For example, in the case
+of an imaging assay, the protocol may start with tissue section staining and end
+with the generation of an OME-TIFF file. The documented protocol should also
+include any image processing steps involved in producing the final OME-TIFF.
+Example: https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1</t>
       </text>
     </comment>
     <comment ref="D1" authorId="1">
       <text>
-        <t>(Required) The specific type of dataset being produced.</t>
+        <t>(Required) The specific type of dataset being produced. Example: RNAseq</t>
       </text>
     </comment>
     <comment ref="E1" authorId="1">
       <text>
-        <t>(Required) The path to the file with the ORCID IDs for all contributors of this
-dataset (e.g., "./extras/contributors.tsv" or "./contributors.tsv"). This is an
-internal metadata field that is just used for ingest.</t>
+        <t>(Required) The name of the file containing the ORCID IDs for all contributors to
+this dataset. Example: ./contributors.csv</t>
       </text>
     </comment>
     <comment ref="F1" authorId="1">
       <text>
-        <t>(Required) The top level directory containing the raw and/or processed data. For
-a single dataset upload this might be "." where as for a data upload containing
-multiple datasets, this would be the directory name for the respective dataset.
-For instance, if the data is within a directory called "TEST001-RK" use syntax
-"./TEST001-RK" for this field. If there are multiple directory levels, use the
-format "./TEST001-RK/Run1/Pass2" in which "Pass2" is the subdirectory where the
-single dataset's data is stored. This is an internal metadata field that is just
-used for ingest.</t>
+        <t>(Required) The top-level directory containing the raw and/or processed data. For
+a single dataset upload, this might be represented as ".", whereas for a data
+upload containing multiple datasets, this would be the directory name for the
+respective dataset. For example, if the data is within a directory named
+"TEST001-RK", use the syntax "./TEST001-RK" for this field. If there are
+multiple directory levels, use the format "./TEST001-RK/Run1/Pass2", where
+"Pass2" is the subdirectory where the single dataset's data is stored. This is
+an internal metadata field used solely for data ingestion. Example: ./TEST001-RK</t>
       </text>
     </comment>
     <comment ref="G1" authorId="1">
       <text>
-        <t>(Required) A lab-generated ID to identify which cells were captured at the same
-time. This would, for example, be an ID to denote which datasets were derived
-from a single 10X Genomics Chromium Controller run. In the case of the 10X
-Controller this could be the chip ID and would allow users the ability to
-determine which samples were processed together in a Chromium controller. It is
-recommended that data providers prefix the ID with the center name, to prevent
-values overlapping across centers.</t>
+        <t>(Required) A lab-assigned identifier used to indicate which cells or nuclei were
+captured together in the same run. For example, in a 10X Genomics Chromium
+Controller workflow, this could be the chip ID used to trace datasets derived
+from a single capture event. This ID helps users identify samples processed
+together on the same device. To avoid conflicts across institutions, it is
+recommended to prefix the ID with the name of the sequencing center. Example:
+Broad_Batch1234</t>
       </text>
     </comment>
     <comment ref="H1" authorId="1">
       <text>
-        <t>(Required) The manufacturer of the instrument used to prepare
-(staining/processing) the sample for the assay. If an automatic slide staining
-method was indicated this field should list the manufacturer of the instrument.</t>
+        <t>(Required) The company that manufactures the instrument used to prepare the
+sample (e.g., for staining or other processing steps) prior to the assay. If the
+instrument was custom-built or developed internally, enter "In-House". If no
+sample preparation occurred, enter "Not applicable". Example: 10X Genomics</t>
       </text>
     </comment>
     <comment ref="I1" authorId="1">
       <text>
-        <t>(Required) Manufacturers of a staining system instrument may offer various
-versions (models) of that instrument with different features. Differences in
-features or sensitivities may be relevant to processing or interpretation of the
-data.</t>
+        <t>(Required) The specific model of the instrument used for sample preparation,
+such as staining. Manufacturers may offer multiple models with varying features
+or sensitivities, which can influence how the sample is processed and how the
+resulting data is interpreted. If no sample preparation occurred, enter "Not
+applicable". Example: Chromium X</t>
       </text>
     </comment>
     <comment ref="J1" authorId="1">
       <text>
-        <t>(Required) The reagent kit used with the preparation instrument.</t>
+        <t>(Required) The reagent kit used in conjunction with the preparation instrument
+for sample processing (e.g., staining or labeling). If the reagent kit was
+prepared using a custom protocol, enter “Custom”. Example: 10X Genomics;
+Chromium Next GEM Chip G Single Cell Kit, 48 rxns; PN 1000120</t>
       </text>
     </comment>
     <comment ref="K1" authorId="1">
       <text>
-        <t>(Required) The number of PCR cycles run after the Chromium Controller step and
-prior to separating the suspension and initiating library construction</t>
+        <t>(Required) The number of PCR cycles performed following the Chromium Controller
+step and before the suspension is separated and library construction begins.
+Example: 7</t>
       </text>
     </comment>
     <comment ref="L1" authorId="1">
       <text>
-        <t>(Required) The string that serves as the definitive identifier for the metadata
-schema version and is readily interpretable by computers for data validation and
+        <t>(Required) The unique string identifier for the metadata specification version,
+which is easily interpretable by computers for purposes of data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
       </text>
     </comment>
@@ -126,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="196">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -152,34 +155,172 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
   </si>
   <si>
+    <t>COMET</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000458</t>
+  </si>
+  <si>
+    <t>Visium (no probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
+  </si>
+  <si>
+    <t>DESI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
+  </si>
+  <si>
+    <t>Confocal</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+  </si>
+  <si>
+    <t>Stereo-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
+  </si>
+  <si>
+    <t>Visium (with probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
+  </si>
+  <si>
+    <t>Molecular Cartography</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
+  </si>
+  <si>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
+  </si>
+  <si>
+    <t>Seq-Scope</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
+  </si>
+  <si>
+    <t>CosMx Transcriptomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
+  </si>
+  <si>
+    <t>CyCIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
+  </si>
+  <si>
+    <t>Light Sheet</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+  </si>
+  <si>
+    <t>seqFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
+  </si>
+  <si>
+    <t>ATACseq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
+  </si>
+  <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
+    <t>Singular Genomics G4X</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
+  </si>
+  <si>
+    <t>Visium HD</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000451</t>
+  </si>
+  <si>
+    <t>MERFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
+  </si>
+  <si>
+    <t>10X Multiome</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
+  </si>
+  <si>
+    <t>4i</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000447</t>
+  </si>
+  <si>
+    <t>PhenoCycler</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
+  </si>
+  <si>
+    <t>Second Harmonic Generation (SHG)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
+  </si>
+  <si>
+    <t>Thick section Multiphoton MxIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
+  </si>
+  <si>
+    <t>CyTOF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+  </si>
+  <si>
+    <t>Olink</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000441</t>
+  </si>
+  <si>
     <t>MIBI</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
   </si>
   <si>
-    <t>Visium (no probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
-  </si>
-  <si>
-    <t>DESI</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
-  </si>
-  <si>
     <t>Auto-fluorescence</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000205</t>
   </si>
   <si>
-    <t>Confocal</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+    <t>FACS</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000440</t>
   </si>
   <si>
     <t>Xenium</t>
@@ -188,36 +329,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000219</t>
   </si>
   <si>
-    <t>Stereo-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
-  </si>
-  <si>
-    <t>Visium (with probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
-  </si>
-  <si>
-    <t>Molecular Cartography</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
-  </si>
-  <si>
-    <t>CosMx</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
-  </si>
-  <si>
-    <t>DBiT-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
-  </si>
-  <si>
     <t>SIMS</t>
   </si>
   <si>
@@ -248,16 +359,10 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
   </si>
   <si>
-    <t>CyCIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
-  </si>
-  <si>
-    <t>Light Sheet</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+    <t>Pixel-seqV2</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000450</t>
   </si>
   <si>
     <t>MALDI</t>
@@ -266,24 +371,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000201</t>
   </si>
   <si>
-    <t>seqFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
-  </si>
-  <si>
     <t>2D Imaging Mass Cytometry</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000296</t>
   </si>
   <si>
-    <t>ATACseq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
-  </si>
-  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -314,18 +407,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000310</t>
   </si>
   <si>
-    <t>Singular Genomics G4X</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
-  </si>
-  <si>
-    <t>MERFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
-  </si>
-  <si>
     <t>LC-MS</t>
   </si>
   <si>
@@ -338,12 +419,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000312</t>
   </si>
   <si>
-    <t>10X Multiome</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
-  </si>
-  <si>
     <t>GeoMx (nCounter)</t>
   </si>
   <si>
@@ -356,34 +431,16 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000311</t>
   </si>
   <si>
-    <t>PhenoCycler</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
-  </si>
-  <si>
-    <t>Second Harmonic Generation (SHG)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
-  </si>
-  <si>
-    <t>Thick section Multiphoton MxIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
-  </si>
-  <si>
     <t>MS Lipidomics</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
   </si>
   <si>
-    <t>CyTOF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+    <t>MPLEx</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000448</t>
   </si>
   <si>
     <t>contributors_path</t>
@@ -578,6 +635,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000250</t>
   </si>
   <si>
+    <t>10x Genomics; Chromium Single Cell B Chip Kit, 16 rxns; PN 1000074</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000462</t>
+  </si>
+  <si>
     <t>10X Genomics; Chromium NextGem Single Cell Multiome ATAC + Gene Expression Reagent Bundle, 4 rxn; PN 1000285</t>
   </si>
   <si>
@@ -647,7 +710,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-04-24T10:53:44-07:00</t>
+    <t>2025-10-21T13:32:33-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -767,42 +830,42 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="L2" t="s" s="13">
-        <v>168</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$41</formula1>
+      <formula1>'dataset_type'!$A$1:$A$50</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_instrument_vendor'!$A$1:$A$9</formula1>
@@ -811,7 +874,7 @@
       <formula1>'preparation_instrument_model'!$A$1:$A$18</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="J2:J1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_kit'!$A$1:$A$11</formula1>
+      <formula1>'preparation_instrument_kit'!$A$1:$A$12</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="between" sqref="K2:K1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-2147483648</formula1>
@@ -826,7 +889,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1158,6 +1221,78 @@
       </c>
       <c r="B41" t="s" s="0">
         <v>85</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>96</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1175,74 +1310,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>91</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>93</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>95</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>97</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>99</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>101</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>103</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>105</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>107</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1260,146 +1395,146 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>110</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>95</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>112</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>114</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>116</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>118</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>120</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>122</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>124</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>126</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>128</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>130</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>132</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>134</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>136</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>138</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>140</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>141</v>
+        <v>159</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>142</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1409,7 +1544,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1417,90 +1552,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>145</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>147</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>149</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>151</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>153</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>155</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>157</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>159</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>161</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>163</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>165</v>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>184</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1524,30 +1667,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>174</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>175</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>